<commit_message>
Allow borrower to remove lender.
</commit_message>
<xml_diff>
--- a/test/map.xlsx
+++ b/test/map.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
   <si>
     <t>0-0</t>
   </si>
@@ -46,24 +46,27 @@
     <t>0-0-03</t>
   </si>
   <si>
+    <t>LoanRequest should allow borrower to remove lender.</t>
+  </si>
+  <si>
+    <t>0-0-04</t>
+  </si>
+  <si>
     <t>LoandRequest should remove signer signature at request.</t>
   </si>
   <si>
-    <t>0-0-04</t>
+    <t>0-0-05</t>
   </si>
   <si>
     <t>LoanRequest should remove lender signature if borrower changes collateral.</t>
   </si>
   <si>
-    <t>0-0-05</t>
+    <t>0-0-06</t>
   </si>
   <si>
     <t>LoanRequest should remove lender signature if borrower changes initial loan value.</t>
   </si>
   <si>
-    <t>0-0-06</t>
-  </si>
-  <si>
     <t>LoanRequest should remove lender signature if borrower changes rate.</t>
   </si>
   <si>
@@ -73,7 +76,7 @@
     <t>LoanRequest should remove lender signature if borrower changes duration.</t>
   </si>
   <si>
-    <t>0-0-08</t>
+    <t>0-0-09</t>
   </si>
   <si>
     <t>LoanRequest should remove lender signature if borrower changes lender.</t>
@@ -246,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -255,6 +258,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -574,15 +583,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="7.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="4.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="100.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="7.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="4.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="100.14785714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -629,14 +638,14 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -675,259 +684,270 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="1"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="1"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="2"/>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+      <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="1"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="2"/>
+      <c r="B24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+      <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="5"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="2"/>
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="A32" s="7"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+      <c r="A33" s="7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="5" t="s">
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+      <c r="A34" s="7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="1"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="3"/>
+      <c r="B34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+      <c r="A35" s="1"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
git add -A! Working copy git add -A!
</commit_message>
<xml_diff>
--- a/test/map.xlsx
+++ b/test/map.xlsx
@@ -249,28 +249,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -589,9 +583,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="7.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="4.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="100.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="7.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="4.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="100.14785714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -623,7 +617,7 @@
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -634,18 +628,18 @@
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="4" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -656,7 +650,7 @@
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -667,7 +661,7 @@
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -678,7 +672,7 @@
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -689,7 +683,7 @@
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -717,7 +711,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1"/>
-      <c r="B12" s="6"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -738,7 +732,7 @@
       <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -749,7 +743,7 @@
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -760,7 +754,7 @@
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -771,13 +765,13 @@
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1"/>
-      <c r="B18" s="6"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
@@ -798,7 +792,7 @@
       <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -848,7 +842,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1"/>
-      <c r="B25" s="6"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
@@ -918,12 +912,12 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="7"/>
-      <c r="B32" s="6"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -934,7 +928,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -946,8 +940,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="1"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="3"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>